<commit_message>
updated app name to healthify in cost estmation and added xlsx and screenshot in the repo.
</commit_message>
<xml_diff>
--- a/Cost_schedule/CostEstimateHealthify.xlsx
+++ b/Cost_schedule/CostEstimateHealthify.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538103\Desktop\GDP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538313\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C720042-B49D-45EA-A4FB-A47608B53CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="1780" yWindow="1780" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -101,16 +110,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Project Name: Healthify-NWMSU</t>
-  </si>
-  <si>
     <t>COST ESTIMATE</t>
+  </si>
+  <si>
+    <t>Project Name: Healthify</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -278,6 +287,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -287,7 +297,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -569,50 +578,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="52.7265625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" customWidth="1"/>
+    <col min="5" max="5" width="29.453125" customWidth="1"/>
+    <col min="7" max="7" width="35.1796875" customWidth="1"/>
+    <col min="8" max="8" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>25</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -629,7 +638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -649,7 +658,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -668,7 +677,7 @@
         <v>24480</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -687,7 +696,7 @@
         <v>91800</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -702,7 +711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -717,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
@@ -732,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -747,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -766,7 +775,7 @@
         <v>85680</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -781,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
@@ -796,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
@@ -815,7 +824,7 @@
         <v>24480</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
@@ -834,7 +843,7 @@
         <v>12240</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -852,21 +861,21 @@
         <v>263160</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="14"/>
       <c r="D18" s="15"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="17"/>
       <c r="E19" s="13"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -882,7 +891,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -890,7 +899,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -898,7 +907,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -906,7 +915,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -914,8 +923,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="11">

</xml_diff>

<commit_message>
added jira work flow screen shot.
</commit_message>
<xml_diff>
--- a/Cost_schedule/CostEstimateHealthify.xlsx
+++ b/Cost_schedule/CostEstimateHealthify.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538313\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538313\Desktop\Healthify-NWMSU\Cost_schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C720042-B49D-45EA-A4FB-A47608B53CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC46A69-EA4C-4EB2-891C-21F6075B28B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1780" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>